<commit_message>
started classed and tsc 2
</commit_message>
<xml_diff>
--- a/zeiterfassung/excel/Zeiterfassung.xlsx
+++ b/zeiterfassung/excel/Zeiterfassung.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Justin\Documents\PROJECTS\Bagjack\BJ-process-automation\zeiterfassung\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4ACD8AF6-85D6-446C-85DD-33F561DAB89A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D0B11BC-F5E4-4302-A88A-0D14FEE8A8B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="23880" yWindow="-120" windowWidth="24240" windowHeight="18240" xr2:uid="{87DF0EE6-B524-4AA6-A647-AE85E584C8D7}"/>
+    <workbookView xWindow="29460" yWindow="585" windowWidth="18000" windowHeight="12945" xr2:uid="{87DF0EE6-B524-4AA6-A647-AE85E584C8D7}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -35,9 +35,27 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
-  <si>
-    <t>ZEIT</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+  <si>
+    <t>Auftrag</t>
+  </si>
+  <si>
+    <t>Kategorie</t>
+  </si>
+  <si>
+    <t>Arbeitschritt</t>
+  </si>
+  <si>
+    <t>Menge</t>
+  </si>
+  <si>
+    <t>Maschiene</t>
+  </si>
+  <si>
+    <t>Arbeitskraft</t>
+  </si>
+  <si>
+    <t>Zeit</t>
   </si>
 </sst>
 </file>
@@ -389,17 +407,35 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E340A213-6FC4-4EE0-A19A-610D4D60AA70}">
-  <dimension ref="C1"/>
+  <dimension ref="A1:G1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="42" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
       <c r="C1" t="s">
-        <v>0</v>
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>